<commit_message>
Rasheed Commit -Fix Employee Middle Name Issue - Fix Employee Import - Other
</commit_message>
<xml_diff>
--- a/public/sample_imports/SampleEmployee.xlsx
+++ b/public/sample_imports/SampleEmployee.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\vs1_cloud_dev\public\sample_imports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="390" windowWidth="27555" windowHeight="12315"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>First Name</t>
   </si>
@@ -37,9 +42,6 @@
     <t>Street</t>
   </si>
   <si>
-    <t>Street2</t>
-  </si>
-  <si>
     <t>State</t>
   </si>
   <si>
@@ -64,20 +66,41 @@
     <t>123 Main Street</t>
   </si>
   <si>
-    <t>Main Street</t>
-  </si>
-  <si>
     <t>New York</t>
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>City/Suburb</t>
+  </si>
+  <si>
+    <t>Brooklyn</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>jane@email.com</t>
+  </si>
+  <si>
+    <t>janesmith</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +232,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -511,7 +542,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -554,12 +585,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -593,6 +626,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -608,6 +642,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -656,7 +693,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -691,7 +728,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -900,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,7 +957,7 @@
     <col min="11" max="11" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,24 +980,27 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
       </c>
       <c r="C2">
         <v>9995551213</v>
@@ -968,29 +1008,74 @@
       <c r="D2">
         <v>9995551213</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
       </c>
       <c r="J2">
         <v>1234</v>
       </c>
       <c r="K2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>9995551213</v>
+      </c>
+      <c r="D3">
+        <v>9995551213</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
         <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>1234</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>